<commit_message>
Wills update in PECO
</commit_message>
<xml_diff>
--- a/data/PECO Jul 20.xlsx
+++ b/data/PECO Jul 20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2286432b\OneDrive - University of Glasgow\R Studio - home folder\Citation network analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marissa\Documents\Citation-Network-Analysis-New\Citation-Network-Analysis-New\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7CA5AC-1C07-46FE-9944-D0C738017B6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293F38CF-92CA-4F76-8DEF-15BA2702E981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PECO Full" sheetId="3" r:id="rId1"/>
@@ -550,9 +550,6 @@
     <t>Huang, J et al. (2014b)</t>
   </si>
   <si>
-    <t>Wills, TA et al. (2016b)</t>
-  </si>
-  <si>
     <t>Ballbe, M et al. (2014)</t>
   </si>
   <si>
@@ -590,6 +587,9 @@
   </si>
   <si>
     <t>ENDs and ENNDS for smoking cessation</t>
+  </si>
+  <si>
+    <t>Wills, TA et al. (2016a)</t>
   </si>
 </sst>
 </file>
@@ -1019,20 +1019,20 @@
       <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="33.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" style="3" customWidth="1"/>
     <col min="4" max="4" width="31" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.81640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="26.81640625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1534,16 +1534,16 @@
         <v>169</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>152</v>
@@ -1552,7 +1552,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>17</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>158</v>
@@ -1682,7 +1682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="AA32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -1950,13 +1950,13 @@
         <v>25</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>103</v>
@@ -1965,7 +1965,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>22</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>77</v>
@@ -2043,21 +2043,21 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>129</v>
@@ -2069,7 +2069,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2095,12 +2095,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>119</v>
@@ -2121,7 +2121,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -2225,12 +2225,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>86</v>
@@ -2242,16 +2242,16 @@
         <v>58</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H46" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="7">
         <v>47</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
         <v>48</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>49</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
         <v>50</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>51</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="7">
         <v>52</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="7">
         <v>53</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -2499,49 +2499,49 @@
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2552,12 +2552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CF7793DA0DEC7646B4067AE33236EE6A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a48280fc6c2b4371bf74abb2bee37b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c55d3ce8-937e-4dcf-883e-347e1ce052b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81c33a3acb51a74fa588efcfe98e5c44" ns3:_="">
     <xsd:import namespace="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
@@ -2689,6 +2683,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2699,22 +2699,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8068956F-FE7C-4286-A5F2-2ED11E40F0B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2732,6 +2716,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F76E9A0E-D7EE-4BF5-A12E-4E5F702CFFF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="c55d3ce8-937e-4dcf-883e-347e1ce052b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2DACEE4-B390-44A7-883A-AFBB4DC509ED}">
   <ds:schemaRefs>

</xml_diff>